<commit_message>
Finally pos tagging the whole dataset.
</commit_message>
<xml_diff>
--- a/results/summary.xlsx
+++ b/results/summary.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12990"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12600" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="99">
   <si>
     <t>Word</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Treebank w/ wordnet and names</t>
+  </si>
+  <si>
+    <t>Brown+Wordnet+Names+COCA</t>
   </si>
 </sst>
 </file>
@@ -702,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +718,7 @@
     <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
@@ -734,8 +737,11 @@
       <c r="F1" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -754,8 +760,11 @@
       <c r="F2" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -774,8 +783,11 @@
       <c r="F3" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -794,8 +806,11 @@
       <c r="F4" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -814,8 +829,11 @@
       <c r="F5" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -834,8 +852,11 @@
       <c r="F6" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -854,8 +875,11 @@
       <c r="F7" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -874,8 +898,11 @@
       <c r="F8" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -894,8 +921,11 @@
       <c r="F9" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -914,8 +944,11 @@
       <c r="F10" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -934,8 +967,11 @@
       <c r="F11" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -954,8 +990,11 @@
       <c r="F12" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -974,8 +1013,11 @@
       <c r="F13" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -994,8 +1036,11 @@
       <c r="F14" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1014,8 +1059,11 @@
       <c r="F15" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1034,8 +1082,11 @@
       <c r="F16" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1054,8 +1105,11 @@
       <c r="F17" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1074,8 +1128,11 @@
       <c r="F18" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1094,8 +1151,11 @@
       <c r="F19" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -1114,8 +1174,11 @@
       <c r="F20" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11</v>
       </c>
@@ -1134,8 +1197,11 @@
       <c r="F21" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
@@ -1154,8 +1220,11 @@
       <c r="F22" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -1174,8 +1243,11 @@
       <c r="F23" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1194,8 +1266,11 @@
       <c r="F24" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1214,8 +1289,11 @@
       <c r="F25" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13</v>
       </c>
@@ -1234,8 +1312,11 @@
       <c r="F26" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14</v>
       </c>
@@ -1254,8 +1335,11 @@
       <c r="F27" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1274,8 +1358,11 @@
       <c r="F28" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -1294,8 +1381,11 @@
       <c r="F29" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1314,8 +1404,11 @@
       <c r="F30" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1334,8 +1427,11 @@
       <c r="F31" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1354,8 +1450,11 @@
       <c r="F32" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>18</v>
       </c>
@@ -1374,8 +1473,11 @@
       <c r="F33" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
@@ -1394,8 +1496,11 @@
       <c r="F34" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>19</v>
       </c>
@@ -1414,8 +1519,11 @@
       <c r="F35" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>19</v>
       </c>
@@ -1434,8 +1542,11 @@
       <c r="F36" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20</v>
       </c>
@@ -1454,8 +1565,11 @@
       <c r="F37" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20</v>
       </c>
@@ -1474,8 +1588,11 @@
       <c r="F38" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20</v>
       </c>
@@ -1494,8 +1611,11 @@
       <c r="F39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>21</v>
       </c>
@@ -1514,8 +1634,11 @@
       <c r="F40" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>21</v>
       </c>
@@ -1534,8 +1657,11 @@
       <c r="F41" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
@@ -1554,8 +1680,11 @@
       <c r="F42" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>22</v>
       </c>
@@ -1574,8 +1703,11 @@
       <c r="F43" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>22</v>
       </c>
@@ -1594,8 +1726,11 @@
       <c r="F44" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>23</v>
       </c>
@@ -1614,8 +1749,11 @@
       <c r="F45" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>23</v>
       </c>
@@ -1634,8 +1772,11 @@
       <c r="F46" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>24</v>
       </c>
@@ -1654,8 +1795,11 @@
       <c r="F47" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>25</v>
       </c>
@@ -1674,8 +1818,11 @@
       <c r="F48" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>26</v>
       </c>
@@ -1694,8 +1841,11 @@
       <c r="F49" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>26</v>
       </c>
@@ -1714,8 +1864,11 @@
       <c r="F50" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>27</v>
       </c>
@@ -1734,8 +1887,11 @@
       <c r="F51" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>28</v>
       </c>
@@ -1754,8 +1910,11 @@
       <c r="F52" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>29</v>
       </c>
@@ -1774,8 +1933,11 @@
       <c r="F53" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>29</v>
       </c>
@@ -1794,8 +1956,11 @@
       <c r="F54" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>30</v>
       </c>
@@ -1814,8 +1979,11 @@
       <c r="F55" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>31</v>
       </c>
@@ -1834,8 +2002,11 @@
       <c r="F56" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>31</v>
       </c>
@@ -1854,8 +2025,11 @@
       <c r="F57" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>32</v>
       </c>
@@ -1874,8 +2048,11 @@
       <c r="F58" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>33</v>
       </c>
@@ -1894,8 +2071,11 @@
       <c r="F59" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>33</v>
       </c>
@@ -1914,8 +2094,11 @@
       <c r="F60" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>34</v>
       </c>
@@ -1934,8 +2117,11 @@
       <c r="F61" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>35</v>
       </c>
@@ -1954,8 +2140,11 @@
       <c r="F62" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>35</v>
       </c>
@@ -1974,8 +2163,11 @@
       <c r="F63" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>36</v>
       </c>
@@ -1994,8 +2186,11 @@
       <c r="F64" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>37</v>
       </c>
@@ -2014,8 +2209,11 @@
       <c r="F65" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>37</v>
       </c>
@@ -2034,8 +2232,11 @@
       <c r="F66" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>38</v>
       </c>
@@ -2054,8 +2255,11 @@
       <c r="F67" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>38</v>
       </c>
@@ -2074,8 +2278,11 @@
       <c r="F68" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>39</v>
       </c>
@@ -2094,8 +2301,11 @@
       <c r="F69" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>39</v>
       </c>
@@ -2114,8 +2324,11 @@
       <c r="F70" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>40</v>
       </c>
@@ -2134,8 +2347,11 @@
       <c r="F71" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>40</v>
       </c>
@@ -2154,8 +2370,11 @@
       <c r="F72" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>40</v>
       </c>
@@ -2174,8 +2393,11 @@
       <c r="F73" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>41</v>
       </c>
@@ -2194,8 +2416,11 @@
       <c r="F74" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>41</v>
       </c>
@@ -2214,8 +2439,11 @@
       <c r="F75" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>42</v>
       </c>
@@ -2234,8 +2462,11 @@
       <c r="F76" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>42</v>
       </c>
@@ -2254,8 +2485,11 @@
       <c r="F77" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>42</v>
       </c>
@@ -2274,8 +2508,11 @@
       <c r="F78" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>42</v>
       </c>
@@ -2292,6 +2529,9 @@
         <v>74</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>